<commit_message>
updating figures and scripts
</commit_message>
<xml_diff>
--- a/Figures/Paper/Abundance-Plot/OrderTaxon.xlsx
+++ b/Figures/Paper/Abundance-Plot/OrderTaxon.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patriciatran/Documents/Github/LakeTanganyika/Figures/Paper/Abundance-Plot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CB80BD-66CE-D84F-BFAC-C2B95B688417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D29D968-06B7-8A4B-B51F-7BD0CC848A2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="460" windowWidth="24920" windowHeight="17860" xr2:uid="{D153EFED-1A48-2A4F-886A-383FE78509BA}"/>
+    <workbookView xWindow="2240" yWindow="460" windowWidth="24900" windowHeight="19200" xr2:uid="{D153EFED-1A48-2A4F-886A-383FE78509BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72831BF0-D182-D544-97CE-199A735DE5EF}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1486,42 +1486,50 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" t="s">
-        <v>148</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="A32" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>164</v>
       </c>
       <c r="G32" s="9">
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="E33" t="s">
+        <v>148</v>
+      </c>
+      <c r="F33" t="s">
+        <v>164</v>
+      </c>
       <c r="G33" s="9">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1529,12 +1537,12 @@
         <v>5</v>
       </c>
       <c r="G34" s="9">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1542,33 +1550,25 @@
         <v>5</v>
       </c>
       <c r="G35" s="9">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E36" t="s">
-        <v>165</v>
-      </c>
-      <c r="F36" t="s">
-        <v>164</v>
-      </c>
       <c r="G36" s="9">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>17</v>
@@ -1578,18 +1578,18 @@
         <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F37" t="s">
         <v>164</v>
       </c>
       <c r="G37" s="9">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>17</v>
@@ -1599,31 +1599,39 @@
         <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="F38" t="s">
         <v>164</v>
       </c>
       <c r="G38" s="9">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="E39" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" t="s">
+        <v>164</v>
+      </c>
       <c r="G39" s="9">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1631,12 +1639,12 @@
         <v>5</v>
       </c>
       <c r="G40" s="9">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1644,12 +1652,12 @@
         <v>5</v>
       </c>
       <c r="G41" s="9">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1657,12 +1665,12 @@
         <v>5</v>
       </c>
       <c r="G42" s="9">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1670,12 +1678,12 @@
         <v>5</v>
       </c>
       <c r="G43" s="9">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1683,33 +1691,25 @@
         <v>5</v>
       </c>
       <c r="G44" s="9">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F45" t="s">
-        <v>164</v>
-      </c>
       <c r="G45" s="9">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>17</v>
@@ -1719,40 +1719,39 @@
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>146</v>
+        <v>42</v>
       </c>
       <c r="F46" t="s">
         <v>164</v>
       </c>
       <c r="G46" s="9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>146</v>
+      </c>
+      <c r="F47" t="s">
+        <v>164</v>
+      </c>
+      <c r="G47" s="9">
         <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F47" s="8" t="str">
-        <f>VLOOKUP(E47,Sheet2!A:B,2,FALSE)</f>
-        <v>CPR</v>
-      </c>
-      <c r="G47" s="9">
-        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>17</v>
@@ -1762,62 +1761,62 @@
         <v>5</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="F48" s="8" t="str">
         <f>VLOOKUP(E48,Sheet2!A:B,2,FALSE)</f>
         <v>CPR</v>
       </c>
       <c r="G48" s="9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F49" s="8" t="str">
+        <f>VLOOKUP(E49,Sheet2!A:B,2,FALSE)</f>
+        <v>CPR</v>
+      </c>
+      <c r="G49" s="9">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="B50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" t="s">
         <v>149</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>164</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G50" s="9">
         <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F50" s="8" t="str">
-        <f>VLOOKUP(E50,Sheet2!A:B,2,FALSE)</f>
-        <v>CPR</v>
-      </c>
-      <c r="G50" s="9">
-        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>17</v>
@@ -1827,19 +1826,19 @@
         <v>5</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="F51" s="8" t="str">
         <f>VLOOKUP(E51,Sheet2!A:B,2,FALSE)</f>
         <v>CPR</v>
       </c>
       <c r="G51" s="9">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>17</v>
@@ -1849,19 +1848,19 @@
         <v>5</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="F52" s="8" t="str">
         <f>VLOOKUP(E52,Sheet2!A:B,2,FALSE)</f>
         <v>CPR</v>
       </c>
       <c r="G52" s="9">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>17</v>
@@ -1871,19 +1870,19 @@
         <v>5</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="F53" s="8" t="str">
         <f>VLOOKUP(E53,Sheet2!A:B,2,FALSE)</f>
         <v>CPR</v>
       </c>
       <c r="G53" s="9">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>17</v>
@@ -1893,40 +1892,41 @@
         <v>5</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F54" s="8" t="str">
         <f>VLOOKUP(E54,Sheet2!A:B,2,FALSE)</f>
         <v>CPR</v>
       </c>
       <c r="G54" s="9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F55" s="8" t="str">
+        <f>VLOOKUP(E55,Sheet2!A:B,2,FALSE)</f>
+        <v>CPR</v>
+      </c>
+      <c r="G55" s="9">
         <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G55" s="9">
-        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>17</v>
@@ -1936,39 +1936,39 @@
         <v>5</v>
       </c>
       <c r="E56" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G56" s="9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="F56" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G56" s="9">
+      <c r="F57" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G57" s="9">
         <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" t="s">
-        <v>153</v>
-      </c>
-      <c r="F57" t="s">
-        <v>164</v>
-      </c>
-      <c r="G57" s="9">
-        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>17</v>
@@ -1978,40 +1978,39 @@
         <v>5</v>
       </c>
       <c r="E58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F58" t="s">
         <v>164</v>
       </c>
       <c r="G58" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>154</v>
+      </c>
+      <c r="F59" t="s">
+        <v>164</v>
+      </c>
+      <c r="G59" s="9">
         <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F59" s="8" t="str">
-        <f>VLOOKUP(E59,Sheet2!A:B,2,FALSE)</f>
-        <v>CPR</v>
-      </c>
-      <c r="G59" s="9">
-        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>17</v>
@@ -2021,19 +2020,19 @@
         <v>5</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F60" s="8" t="str">
         <f>VLOOKUP(E60,Sheet2!A:B,2,FALSE)</f>
         <v>CPR</v>
       </c>
       <c r="G60" s="9">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>17</v>
@@ -2043,61 +2042,62 @@
         <v>5</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="F61" s="8" t="str">
         <f>VLOOKUP(E61,Sheet2!A:B,2,FALSE)</f>
         <v>CPR</v>
       </c>
       <c r="G61" s="9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F62" s="8" t="str">
+        <f>VLOOKUP(E62,Sheet2!A:B,2,FALSE)</f>
+        <v>CPR</v>
+      </c>
+      <c r="G62" s="9">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="B63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
         <v>155</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F63" t="s">
         <v>164</v>
       </c>
-      <c r="G62" s="9">
+      <c r="G63" s="9">
         <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="F63" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="G63" s="9">
-        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>17</v>
@@ -2107,98 +2107,98 @@
         <v>5</v>
       </c>
       <c r="E64" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G64" s="9">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="F64" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G64" s="9">
+      <c r="F65" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G65" s="9">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="B66" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
         <v>158</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F66" t="s">
         <v>164</v>
       </c>
-      <c r="G65" s="9">
+      <c r="G66" s="9">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="10" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B66" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" s="11" t="s">
+      <c r="B67" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="F66" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G66" s="9">
+      <c r="F67" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G67" s="9">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="7" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B67" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E67" s="8" t="s">
+      <c r="B68" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F67" s="8" t="str">
-        <f>VLOOKUP(E67,Sheet2!A:B,2,FALSE)</f>
+      <c r="F68" s="8" t="str">
+        <f>VLOOKUP(E68,Sheet2!A:B,2,FALSE)</f>
         <v>CPR</v>
       </c>
-      <c r="G67" s="9">
+      <c r="G68" s="9">
         <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G68" s="9">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>